<commit_message>
San Diego changes and edits.
</commit_message>
<xml_diff>
--- a/docs/Gravity Loads.xlsx
+++ b/docs/Gravity Loads.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wroser\Documents\Code Workshop\3D Model 2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\wfros\Documents\Will\College\Code Workshop\Model_10_Story\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F048DDC8-7C7A-4C48-86DF-079A9F063A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF35CCB-B9E3-4E39-895D-9D45B8BE55BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Total Loads" sheetId="1" r:id="rId1"/>
-    <sheet name="Voronoi Gravity" sheetId="2" r:id="rId2"/>
+    <sheet name="Export Data" sheetId="4" r:id="rId1"/>
+    <sheet name="Total Loads" sheetId="1" r:id="rId2"/>
+    <sheet name="Import Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Voronoi Gravity" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
   <si>
     <t>Floor</t>
   </si>
@@ -93,14 +95,6 @@
   </si>
   <si>
     <t>Tributary Floor Height (ft)</t>
-  </si>
-  <si>
-    <t>both CLT
-(kip)</t>
-  </si>
-  <si>
-    <t>both MPP
-(kip)</t>
   </si>
   <si>
     <t>All Walls
@@ -184,6 +178,128 @@
   </si>
   <si>
     <t>Fy</t>
+  </si>
+  <si>
+    <t>each CLT
+(kip)</t>
+  </si>
+  <si>
+    <t>each MPP
+(kip)</t>
+  </si>
+  <si>
+    <t>Mass Update 01-28-2022.docx</t>
+  </si>
+  <si>
+    <t>Last updated 12-13-2022.</t>
+  </si>
+  <si>
+    <t>Table 1.</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Calculated with Wall Weight</t>
+  </si>
+  <si>
+    <t>Calculated without Wall Weight</t>
+  </si>
+  <si>
+    <t>Diaphragm</t>
+  </si>
+  <si>
+    <t>Beams</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>CLT Walls</t>
+  </si>
+  <si>
+    <t>MPP Walls</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Stairs</t>
+  </si>
+  <si>
+    <t>NS Walls</t>
+  </si>
+  <si>
+    <t>Mass Plates</t>
+  </si>
+  <si>
+    <t>w/o Walls</t>
+  </si>
+  <si>
+    <t>Walls Only</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Xm</t>
+  </si>
+  <si>
+    <t>Ym</t>
+  </si>
+  <si>
+    <t>Io</t>
+  </si>
+  <si>
+    <t>k/floor</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>k in s2</t>
+  </si>
+  <si>
+    <t>pcf</t>
+  </si>
+  <si>
+    <t>kli</t>
+  </si>
+  <si>
+    <t>klf</t>
+  </si>
+  <si>
+    <t>Values to Export to OpenSees Model</t>
+  </si>
+  <si>
+    <t>eleProperties</t>
+  </si>
+  <si>
+    <t>CLT</t>
+  </si>
+  <si>
+    <t>MPP</t>
+  </si>
+  <si>
+    <t>Mass (kip*s²/in)</t>
+  </si>
+  <si>
+    <t>Center of Mass, Mass, and Inertia</t>
+  </si>
+  <si>
+    <t>Floor Plan</t>
   </si>
 </sst>
 </file>
@@ -240,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +366,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -307,7 +429,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,13 +477,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1807,23 +1933,282 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC31B580-7BB8-426F-82AF-EF6408344079}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="26">
+        <f>'Total Loads'!H5/32.2/12</f>
+        <v>7.8429946214927311E-5</v>
+      </c>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="26">
+        <f>'Total Loads'!H6/32.2/12</f>
+        <v>5.3911559862023196E-5</v>
+      </c>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="25">
+        <f>'Import Data'!G8</f>
+        <v>188.6</v>
+      </c>
+      <c r="C11" s="25">
+        <f>'Import Data'!H8</f>
+        <v>-125.4</v>
+      </c>
+      <c r="D11" s="25">
+        <f>'Import Data'!W7/32.2/12</f>
+        <v>0.1472567287784679</v>
+      </c>
+      <c r="E11" s="25">
+        <f>'Import Data'!I8/32.2/12</f>
+        <v>12.502587991718427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="25">
+        <f>'Import Data'!G9</f>
+        <v>194.7</v>
+      </c>
+      <c r="C12" s="25">
+        <f>'Import Data'!H9</f>
+        <v>-135.9</v>
+      </c>
+      <c r="D12" s="25">
+        <f>'Import Data'!W8/32.2/12</f>
+        <v>0.1400103519668737</v>
+      </c>
+      <c r="E12" s="25">
+        <f>'Import Data'!I9/32.2/12</f>
+        <v>10.986024844720497</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="25">
+        <f>'Import Data'!G10</f>
+        <v>199</v>
+      </c>
+      <c r="C13" s="25">
+        <f>'Import Data'!H10</f>
+        <v>-144.30000000000001</v>
+      </c>
+      <c r="D13" s="25">
+        <f>'Import Data'!W9/32.2/12</f>
+        <v>0.11697722567287783</v>
+      </c>
+      <c r="E13" s="25">
+        <f>'Import Data'!I10/32.2/12</f>
+        <v>7.9244306418219459</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="25">
+        <f>'Import Data'!G11</f>
+        <v>191.2</v>
+      </c>
+      <c r="C14" s="25">
+        <f>'Import Data'!H11</f>
+        <v>-139.9</v>
+      </c>
+      <c r="D14" s="25">
+        <f>'Import Data'!W10/32.2/12</f>
+        <v>0.10998964803312627</v>
+      </c>
+      <c r="E14" s="25">
+        <f>'Import Data'!I11/32.2/12</f>
+        <v>6.2862318840579698</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="25">
+        <f>'Import Data'!G12</f>
+        <v>191.4</v>
+      </c>
+      <c r="C15" s="25">
+        <f>'Import Data'!H12</f>
+        <v>-144.6</v>
+      </c>
+      <c r="D15" s="25">
+        <f>'Import Data'!W11/32.2/12</f>
+        <v>0.12422360248447205</v>
+      </c>
+      <c r="E15" s="25">
+        <f>'Import Data'!I12/32.2/12</f>
+        <v>6.537267080745341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="25">
+        <f>'Import Data'!G13</f>
+        <v>191.1</v>
+      </c>
+      <c r="C16" s="25">
+        <f>'Import Data'!H13</f>
+        <v>-135.19999999999999</v>
+      </c>
+      <c r="D16" s="25">
+        <f>'Import Data'!W12/32.2/12</f>
+        <v>0.10895445134575567</v>
+      </c>
+      <c r="E16" s="25">
+        <f>'Import Data'!I13/32.2/12</f>
+        <v>6.1387163561076603</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="25">
+        <f>'Import Data'!G14</f>
+        <v>192</v>
+      </c>
+      <c r="C17" s="25">
+        <f>'Import Data'!H14</f>
+        <v>-135.69999999999999</v>
+      </c>
+      <c r="D17" s="25">
+        <f>'Import Data'!W13/32.2/12</f>
+        <v>0.11853002070393372</v>
+      </c>
+      <c r="E17" s="25">
+        <f>'Import Data'!I14/32.2/12</f>
+        <v>6.9073498964803308</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="25">
+        <f>'Import Data'!G15</f>
+        <v>192</v>
+      </c>
+      <c r="C18" s="25">
+        <f>'Import Data'!H15</f>
+        <v>-134.6</v>
+      </c>
+      <c r="D18" s="25">
+        <f>'Import Data'!W14/32.2/12</f>
+        <v>0.11464803312629397</v>
+      </c>
+      <c r="E18" s="25">
+        <f>'Import Data'!I15/32.2/12</f>
+        <v>6.8840579710144922</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="25">
+        <f>'Import Data'!G16</f>
+        <v>192</v>
+      </c>
+      <c r="C19" s="25">
+        <f>'Import Data'!H16</f>
+        <v>-137.4</v>
+      </c>
+      <c r="D19" s="25">
+        <f>'Import Data'!W15/32.2/12</f>
+        <v>0.1089544513457557</v>
+      </c>
+      <c r="E19" s="25">
+        <f>'Import Data'!I16/32.2/12</f>
+        <v>6.70807453416149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="25">
+        <f>'Import Data'!G17</f>
+        <v>192</v>
+      </c>
+      <c r="C20" s="25">
+        <f>'Import Data'!H17</f>
+        <v>-135.80000000000001</v>
+      </c>
+      <c r="D20" s="25">
+        <f>'Import Data'!W16/32.2/12</f>
+        <v>8.9544513457556929E-2</v>
+      </c>
+      <c r="E20" s="25">
+        <f>'Import Data'!I17/32.2/12</f>
+        <v>5.9575569358178049</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A3:K24"/>
+  <dimension ref="A3:N26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1839,12 +2224,12 @@
       <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1864,12 +2249,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="12">
-        <v>36</v>
+        <v>36.130000000000003</v>
       </c>
       <c r="D5" s="13">
         <v>117.125</v>
@@ -1883,19 +2268,19 @@
       </c>
       <c r="G5" s="3">
         <f>C5/144*F5</f>
-        <v>362.35546875</v>
+        <v>363.66397460937503</v>
       </c>
       <c r="H5" s="15">
         <f>G5/12/1000</f>
-        <v>3.0196289062499999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3.0305331217447919E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="12">
-        <v>37.200000000000003</v>
+        <v>37.270000000000003</v>
       </c>
       <c r="D6" s="13">
         <v>105.125</v>
@@ -1909,14 +2294,14 @@
       </c>
       <c r="G6" s="3">
         <f>C6/144*F6</f>
-        <v>249.50761718750002</v>
+        <v>249.97712076822921</v>
       </c>
       <c r="H6" s="15">
         <f>G6/12/1000</f>
-        <v>2.079230143229167E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>2.0831426730685765E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
@@ -1924,52 +2309,57 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="F11" s="22">
+      <c r="F11" s="21">
         <f>13/2</f>
         <v>6.5</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="14">
         <f>(12*$F11)*($H$5)</f>
-        <v>2.3553105468749997</v>
+        <v>2.3638158349609375</v>
       </c>
       <c r="I11" s="14">
         <f>(12*$F11)*($H$6)</f>
-        <v>1.6217995117187503</v>
+        <v>1.6248512849934897</v>
       </c>
       <c r="J11" s="11">
         <f>2*H11+2*I11</f>
-        <v>7.9542201171875</v>
-      </c>
-      <c r="K11" s="11">
-        <f>SUM(F11,B11)</f>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.9773342399088545</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="M11">
+        <f>H11*2</f>
+        <v>4.727631669921875</v>
+      </c>
+      <c r="N11">
+        <f>I11*2</f>
+        <v>3.2497025699869795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -1977,29 +2367,37 @@
         <v>56.988490816208198</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <f>6.5+5.5</f>
         <v>12</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="14">
         <f t="shared" ref="H12:H21" si="0">(12*$F12)*($H$5)</f>
-        <v>4.3482656249999998</v>
+        <v>4.3639676953125006</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" ref="I12:I21" si="1">(12*$F12)*($H$6)</f>
-        <v>2.9940914062500004</v>
+        <v>2.9997254492187504</v>
       </c>
       <c r="J12" s="11">
         <f t="shared" ref="J12:J21" si="2">2*H12+2*I12</f>
-        <v>14.684714062499999</v>
+        <v>14.727386289062501</v>
       </c>
       <c r="K12" s="11">
-        <f t="shared" ref="K12:K21" si="3">SUM(F12,B12)</f>
-        <v>68.988490816208198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <f>SUM(J12,B12)</f>
+        <v>71.715877105270692</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:M21" si="3">H12*2</f>
+        <v>8.7279353906250012</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12:N21" si="4">I12*2</f>
+        <v>5.9994508984375008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -2007,28 +2405,36 @@
         <v>54.148361192249887</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>11</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="21"/>
       <c r="H13" s="14">
-        <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <f>(12*$F13)*($H$5)</f>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I13" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J13" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K13" s="11">
+        <f t="shared" ref="K13:K21" si="5">SUM(J13,B13)</f>
+        <v>67.648465290557183</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="3"/>
-        <v>65.148361192249894</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -2036,28 +2442,36 @@
         <v>45.325434576644867</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>11</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="14">
-        <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <f>(12*$F14)*($H$5)</f>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J14" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K14" s="11">
+        <f t="shared" si="5"/>
+        <v>58.825538674952156</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="3"/>
-        <v>56.325434576644867</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>5</v>
       </c>
@@ -2065,28 +2479,36 @@
         <v>42.59826794664486</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>11</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="14">
         <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I15" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J15" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K15" s="11">
+        <f t="shared" si="5"/>
+        <v>56.098372044952157</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="3"/>
-        <v>53.59826794664486</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>6</v>
       </c>
@@ -2094,28 +2516,36 @@
         <v>48.077825718329116</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="F16" s="22">
+      <c r="F16" s="21">
         <v>11</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="14">
         <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I16" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J16" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K16" s="11">
+        <f t="shared" si="5"/>
+        <v>61.577929816636413</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="3"/>
-        <v>59.077825718329116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>7</v>
       </c>
@@ -2123,28 +2553,36 @@
         <v>42.101681913713733</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="F17" s="22">
+      <c r="F17" s="21">
         <v>11</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="14">
         <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I17" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J17" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K17" s="11">
+        <f t="shared" si="5"/>
+        <v>55.601786012021023</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="3"/>
-        <v>53.101681913713733</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>8</v>
       </c>
@@ -2152,28 +2590,36 @@
         <v>45.724234295823827</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="F18" s="22">
+      <c r="F18" s="21">
         <v>11</v>
       </c>
-      <c r="G18" s="22"/>
+      <c r="G18" s="21"/>
       <c r="H18" s="14">
         <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I18" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J18" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K18" s="11">
+        <f t="shared" si="5"/>
+        <v>59.224338394131124</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="3"/>
-        <v>56.724234295823827</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>9</v>
       </c>
@@ -2181,28 +2627,36 @@
         <v>44.224234295823827</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="F19" s="22">
+      <c r="F19" s="21">
         <v>11</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="14">
         <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J19" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K19" s="11">
+        <f t="shared" si="5"/>
+        <v>57.724338394131124</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="3"/>
-        <v>55.224234295823827</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>10</v>
       </c>
@@ -2210,28 +2664,36 @@
         <v>42.034234295823829</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <v>11</v>
       </c>
-      <c r="G20" s="22"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="14">
         <f t="shared" si="0"/>
-        <v>3.9859101562500001</v>
+        <v>4.0003037207031253</v>
       </c>
       <c r="I20" s="14">
         <f t="shared" si="1"/>
-        <v>2.7445837890625007</v>
+        <v>2.7497483284505209</v>
       </c>
       <c r="J20" s="11">
         <f t="shared" si="2"/>
-        <v>13.460987890625002</v>
+        <v>13.500104098307293</v>
       </c>
       <c r="K20" s="11">
+        <f t="shared" si="5"/>
+        <v>55.534338394131126</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="3"/>
-        <v>53.034234295823829</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.0006074414062507</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>5.4994966569010417</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -2239,28 +2701,36 @@
         <v>34.477230064053003</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="F21" s="22">
+      <c r="F21" s="21">
         <v>8</v>
       </c>
-      <c r="G21" s="22"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="14">
         <f t="shared" si="0"/>
-        <v>2.8988437500000002</v>
+        <v>2.9093117968750004</v>
       </c>
       <c r="I21" s="14">
         <f t="shared" si="1"/>
-        <v>1.9960609375000002</v>
+        <v>1.9998169661458336</v>
       </c>
       <c r="J21" s="11">
         <f t="shared" si="2"/>
-        <v>9.7898093750000008</v>
+        <v>9.818257526041668</v>
       </c>
       <c r="K21" s="11">
+        <f t="shared" si="5"/>
+        <v>44.295487590094673</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="3"/>
-        <v>42.477230064053003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.8186235937500008</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>3.9996339322916672</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
@@ -2271,34 +2741,46 @@
       <c r="C22" s="3"/>
       <c r="H22" s="16">
         <f>SUM(H11:H21)</f>
-        <v>41.489701171874998</v>
+        <v>41.639525092773447</v>
       </c>
       <c r="I22" s="16">
-        <f t="shared" ref="I22:K22" si="4">SUM(I11:I21)</f>
-        <v>28.568622167968755</v>
+        <f t="shared" ref="I22:K22" si="6">SUM(I11:I21)</f>
+        <v>28.622380327962244</v>
       </c>
       <c r="J22" s="16">
-        <f t="shared" si="4"/>
-        <v>140.11664667968753</v>
+        <f t="shared" si="6"/>
+        <v>140.52381084147135</v>
       </c>
       <c r="K22" s="11">
-        <f t="shared" si="4"/>
-        <v>570.19999511531501</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
+        <f>SUM(J22,B22)</f>
+        <v>596.22380595678646</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
       <c r="K24" s="17">
         <f>K22</f>
-        <v>570.19999511531501</v>
-      </c>
+        <v>596.22380595678646</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="F10:G10"/>
@@ -2307,12 +2789,6 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2320,21 +2796,1503 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F7A999-871F-4469-8719-624E0FAAA706}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="B2:AD29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U7" sqref="U7:U14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5" t="s">
+        <v>64</v>
+      </c>
+      <c r="X5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>73</v>
+      </c>
+      <c r="R6" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" t="s">
+        <v>73</v>
+      </c>
+      <c r="T6" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>16.7</v>
+      </c>
+      <c r="M7">
+        <v>4.3</v>
+      </c>
+      <c r="N7">
+        <v>7.5</v>
+      </c>
+      <c r="O7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>6.9</v>
+      </c>
+      <c r="R7">
+        <v>6.7</v>
+      </c>
+      <c r="S7">
+        <v>14.8</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>71.7</v>
+      </c>
+      <c r="W7">
+        <f>SUM(L7:N7,Q7:T7)</f>
+        <v>56.900000000000006</v>
+      </c>
+      <c r="X7">
+        <f>SUM(O7:P7)</f>
+        <v>14.7</v>
+      </c>
+      <c r="Z7">
+        <f>G8</f>
+        <v>188.6</v>
+      </c>
+      <c r="AA7">
+        <f>H8</f>
+        <v>-125.4</v>
+      </c>
+      <c r="AB7">
+        <f>SUM(L7:N7,Q7:T7)/32.2/12</f>
+        <v>0.1472567287784679</v>
+      </c>
+      <c r="AC7">
+        <f>I8/32.2/12</f>
+        <v>12.502587991718427</v>
+      </c>
+    </row>
+    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>71.7</v>
+      </c>
+      <c r="D8">
+        <v>189.7</v>
+      </c>
+      <c r="E8">
+        <v>-115.9</v>
+      </c>
+      <c r="F8">
+        <v>5944</v>
+      </c>
+      <c r="G8">
+        <v>188.6</v>
+      </c>
+      <c r="H8">
+        <v>-125.4</v>
+      </c>
+      <c r="I8">
+        <v>4831</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>16.7</v>
+      </c>
+      <c r="M8">
+        <v>4.3</v>
+      </c>
+      <c r="N8">
+        <v>6.9</v>
+      </c>
+      <c r="O8">
+        <v>8</v>
+      </c>
+      <c r="P8">
+        <v>5.5</v>
+      </c>
+      <c r="Q8">
+        <v>6.9</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
+      </c>
+      <c r="S8">
+        <v>11.3</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="W8">
+        <f>SUM(L8:N8,Q8:T8)</f>
+        <v>54.099999999999994</v>
+      </c>
+      <c r="X8">
+        <f>SUM(O8:P8)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z8">
+        <f>G9</f>
+        <v>194.7</v>
+      </c>
+      <c r="AA8">
+        <f>H9</f>
+        <v>-135.9</v>
+      </c>
+      <c r="AB8">
+        <f>SUM(L8:N8,Q8:T8)/32.2/12</f>
+        <v>0.1400103519668737</v>
+      </c>
+      <c r="AC8">
+        <f>I9/32.2/12</f>
+        <v>10.986024844720497</v>
+      </c>
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="D9">
+        <v>194.3</v>
+      </c>
+      <c r="E9">
+        <v>-123.9</v>
+      </c>
+      <c r="F9">
+        <v>5305</v>
+      </c>
+      <c r="G9">
+        <v>194.7</v>
+      </c>
+      <c r="H9">
+        <v>-135.9</v>
+      </c>
+      <c r="I9">
+        <v>4245</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>14.2</v>
+      </c>
+      <c r="M9">
+        <v>4.3</v>
+      </c>
+      <c r="N9">
+        <v>6.9</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9">
+        <v>5.5</v>
+      </c>
+      <c r="Q9">
+        <v>6.9</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="S9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>58.8</v>
+      </c>
+      <c r="W9">
+        <f>SUM(L9:N9,Q9:T9)</f>
+        <v>45.199999999999996</v>
+      </c>
+      <c r="X9">
+        <f>SUM(O9:P9)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z9">
+        <f>G10</f>
+        <v>199</v>
+      </c>
+      <c r="AA9">
+        <f>H10</f>
+        <v>-144.30000000000001</v>
+      </c>
+      <c r="AB9">
+        <f>SUM(L9:N9,Q9:T9)/32.2/12</f>
+        <v>0.11697722567287783</v>
+      </c>
+      <c r="AC9">
+        <f>I10/32.2/12</f>
+        <v>7.9244306418219459</v>
+      </c>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>58.8</v>
+      </c>
+      <c r="D10">
+        <v>197.3</v>
+      </c>
+      <c r="E10">
+        <v>-128.1</v>
+      </c>
+      <c r="F10">
+        <v>4137</v>
+      </c>
+      <c r="G10">
+        <v>199</v>
+      </c>
+      <c r="H10">
+        <v>-144.30000000000001</v>
+      </c>
+      <c r="I10">
+        <v>3062</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>14.2</v>
+      </c>
+      <c r="M10">
+        <v>4.3</v>
+      </c>
+      <c r="N10">
+        <v>6.9</v>
+      </c>
+      <c r="O10">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <v>5.5</v>
+      </c>
+      <c r="Q10">
+        <v>6.9</v>
+      </c>
+      <c r="R10">
+        <v>7.9</v>
+      </c>
+      <c r="S10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>56.1</v>
+      </c>
+      <c r="W10">
+        <f>SUM(L10:N10,Q10:T10)</f>
+        <v>42.499999999999993</v>
+      </c>
+      <c r="X10">
+        <f>SUM(O10:P10)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z10">
+        <f>G11</f>
+        <v>191.2</v>
+      </c>
+      <c r="AA10">
+        <f>H11</f>
+        <v>-139.9</v>
+      </c>
+      <c r="AB10">
+        <f>SUM(L10:N10,Q10:T10)/32.2/12</f>
+        <v>0.10998964803312627</v>
+      </c>
+      <c r="AC10">
+        <f>I11/32.2/12</f>
+        <v>6.2862318840579698</v>
+      </c>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>56.1</v>
+      </c>
+      <c r="D11">
+        <v>191.7</v>
+      </c>
+      <c r="E11">
+        <v>-124.3</v>
+      </c>
+      <c r="F11">
+        <v>3490</v>
+      </c>
+      <c r="G11">
+        <v>191.2</v>
+      </c>
+      <c r="H11">
+        <v>-139.9</v>
+      </c>
+      <c r="I11">
+        <v>2429</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>14</v>
+      </c>
+      <c r="M11">
+        <v>4.3</v>
+      </c>
+      <c r="N11">
+        <v>6.9</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>5.5</v>
+      </c>
+      <c r="Q11">
+        <v>6.9</v>
+      </c>
+      <c r="R11">
+        <v>7.8</v>
+      </c>
+      <c r="S11">
+        <v>8.1</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>61.5</v>
+      </c>
+      <c r="W11">
+        <f>SUM(L11:N11,Q11:T11)</f>
+        <v>48</v>
+      </c>
+      <c r="X11">
+        <f>SUM(O11:P11)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z11">
+        <f>G12</f>
+        <v>191.4</v>
+      </c>
+      <c r="AA11">
+        <f>H12</f>
+        <v>-144.6</v>
+      </c>
+      <c r="AB11">
+        <f>SUM(L11:N11,Q11:T11)/32.2/12</f>
+        <v>0.12422360248447205</v>
+      </c>
+      <c r="AC11">
+        <f>I12/32.2/12</f>
+        <v>6.537267080745341</v>
+      </c>
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>61.5</v>
+      </c>
+      <c r="D12">
+        <v>191.8</v>
+      </c>
+      <c r="E12">
+        <v>-129.1</v>
+      </c>
+      <c r="F12">
+        <v>3604</v>
+      </c>
+      <c r="G12">
+        <v>191.4</v>
+      </c>
+      <c r="H12">
+        <v>-144.6</v>
+      </c>
+      <c r="I12">
+        <v>2526</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>13.9</v>
+      </c>
+      <c r="M12">
+        <v>4.3</v>
+      </c>
+      <c r="N12">
+        <v>6.9</v>
+      </c>
+      <c r="O12">
+        <v>8</v>
+      </c>
+      <c r="P12">
+        <v>5.5</v>
+      </c>
+      <c r="Q12">
+        <v>6.9</v>
+      </c>
+      <c r="R12">
+        <v>7.8</v>
+      </c>
+      <c r="S12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>55.6</v>
+      </c>
+      <c r="W12">
+        <f>SUM(L12:N12,Q12:T12)</f>
+        <v>42.099999999999994</v>
+      </c>
+      <c r="X12">
+        <f>SUM(O12:P12)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z12">
+        <f>G13</f>
+        <v>191.1</v>
+      </c>
+      <c r="AA12">
+        <f>H13</f>
+        <v>-135.19999999999999</v>
+      </c>
+      <c r="AB12">
+        <f>SUM(L12:N12,Q12:T12)/32.2/12</f>
+        <v>0.10895445134575567</v>
+      </c>
+      <c r="AC12">
+        <f>I13/32.2/12</f>
+        <v>6.1387163561076603</v>
+      </c>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>55.6</v>
+      </c>
+      <c r="D13">
+        <v>191.6</v>
+      </c>
+      <c r="E13">
+        <v>-120.9</v>
+      </c>
+      <c r="F13">
+        <v>3423</v>
+      </c>
+      <c r="G13">
+        <v>191.1</v>
+      </c>
+      <c r="H13">
+        <v>-135.19999999999999</v>
+      </c>
+      <c r="I13">
+        <v>2372</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="M13">
+        <v>5.2</v>
+      </c>
+      <c r="N13">
+        <v>6.9</v>
+      </c>
+      <c r="O13">
+        <v>8</v>
+      </c>
+      <c r="P13">
+        <v>5.5</v>
+      </c>
+      <c r="Q13">
+        <v>6.9</v>
+      </c>
+      <c r="R13">
+        <v>7.8</v>
+      </c>
+      <c r="S13">
+        <v>1.9</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>59.2</v>
+      </c>
+      <c r="W13">
+        <f>SUM(L13:N13,Q13:T13)</f>
+        <v>45.8</v>
+      </c>
+      <c r="X13">
+        <f>SUM(O13:P13)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z13">
+        <f>G14</f>
+        <v>192</v>
+      </c>
+      <c r="AA13">
+        <f>H14</f>
+        <v>-135.69999999999999</v>
+      </c>
+      <c r="AB13">
+        <f>SUM(L13:N13,Q13:T13)/32.2/12</f>
+        <v>0.11853002070393372</v>
+      </c>
+      <c r="AC13">
+        <f>I14/32.2/12</f>
+        <v>6.9073498964803308</v>
+      </c>
+    </row>
+    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>59.2</v>
+      </c>
+      <c r="D14">
+        <v>192.3</v>
+      </c>
+      <c r="E14">
+        <v>-122.1</v>
+      </c>
+      <c r="F14">
+        <v>3723</v>
+      </c>
+      <c r="G14">
+        <v>192</v>
+      </c>
+      <c r="H14">
+        <v>-135.69999999999999</v>
+      </c>
+      <c r="I14">
+        <v>2669</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="M14">
+        <v>5.2</v>
+      </c>
+      <c r="N14">
+        <v>6.9</v>
+      </c>
+      <c r="O14">
+        <v>8</v>
+      </c>
+      <c r="P14">
+        <v>5.5</v>
+      </c>
+      <c r="Q14">
+        <v>6.9</v>
+      </c>
+      <c r="R14">
+        <v>6.3</v>
+      </c>
+      <c r="S14">
+        <v>1.9</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>57.7</v>
+      </c>
+      <c r="W14">
+        <f>SUM(L14:N14,Q14:T14)</f>
+        <v>44.3</v>
+      </c>
+      <c r="X14">
+        <f>SUM(O14:P14)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z14">
+        <f>G15</f>
+        <v>192</v>
+      </c>
+      <c r="AA14">
+        <f>H15</f>
+        <v>-134.6</v>
+      </c>
+      <c r="AB14">
+        <f>SUM(L14:N14,Q14:T14)/32.2/12</f>
+        <v>0.11464803312629397</v>
+      </c>
+      <c r="AC14">
+        <f>I15/32.2/12</f>
+        <v>6.8840579710144922</v>
+      </c>
+    </row>
+    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>57.7</v>
+      </c>
+      <c r="D15">
+        <v>192.3</v>
+      </c>
+      <c r="E15">
+        <v>-120.9</v>
+      </c>
+      <c r="F15">
+        <v>3711</v>
+      </c>
+      <c r="G15">
+        <v>192</v>
+      </c>
+      <c r="H15">
+        <v>-134.6</v>
+      </c>
+      <c r="I15">
+        <v>2660</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="M15">
+        <v>5.2</v>
+      </c>
+      <c r="N15">
+        <v>6.9</v>
+      </c>
+      <c r="O15">
+        <v>8</v>
+      </c>
+      <c r="P15">
+        <v>5.5</v>
+      </c>
+      <c r="Q15">
+        <v>6.9</v>
+      </c>
+      <c r="R15">
+        <v>6</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>55.5</v>
+      </c>
+      <c r="W15">
+        <f>SUM(L15:N15,Q15:T15)</f>
+        <v>42.1</v>
+      </c>
+      <c r="X15">
+        <f>SUM(O15:P15)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Z15">
+        <f>G16</f>
+        <v>192</v>
+      </c>
+      <c r="AA15">
+        <f>H16</f>
+        <v>-137.4</v>
+      </c>
+      <c r="AB15">
+        <f>SUM(L15:N15,Q15:T15)/32.2/12</f>
+        <v>0.1089544513457557</v>
+      </c>
+      <c r="AC15">
+        <f>I16/32.2/12</f>
+        <v>6.70807453416149</v>
+      </c>
+    </row>
+    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>55.5</v>
+      </c>
+      <c r="D16">
+        <v>192.3</v>
+      </c>
+      <c r="E16">
+        <v>-122.3</v>
+      </c>
+      <c r="F16">
+        <v>3648</v>
+      </c>
+      <c r="G16">
+        <v>192</v>
+      </c>
+      <c r="H16">
+        <v>-137.4</v>
+      </c>
+      <c r="I16">
+        <v>2592</v>
+      </c>
+      <c r="K16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="M16">
+        <v>5.2</v>
+      </c>
+      <c r="N16">
+        <v>3.5</v>
+      </c>
+      <c r="O16">
+        <v>5.8</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16">
+        <v>5.2</v>
+      </c>
+      <c r="R16">
+        <v>3.6</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>44.3</v>
+      </c>
+      <c r="W16">
+        <f>SUM(L16:N16,Q16:T16)</f>
+        <v>34.6</v>
+      </c>
+      <c r="X16">
+        <f>SUM(O16:P16)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="Z16">
+        <f>G17</f>
+        <v>192</v>
+      </c>
+      <c r="AA16">
+        <f>H17</f>
+        <v>-135.80000000000001</v>
+      </c>
+      <c r="AB16">
+        <f>SUM(L16:N16,Q16:T16)/32.2/12</f>
+        <v>8.9544513457556929E-2</v>
+      </c>
+      <c r="AC16">
+        <f>I17/32.2/12</f>
+        <v>5.9575569358178049</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>44.3</v>
+      </c>
+      <c r="D17">
+        <v>192.2</v>
+      </c>
+      <c r="E17">
+        <v>-123.4</v>
+      </c>
+      <c r="F17">
+        <v>3020</v>
+      </c>
+      <c r="G17">
+        <v>192</v>
+      </c>
+      <c r="H17">
+        <v>-135.80000000000001</v>
+      </c>
+      <c r="I17">
+        <v>2302</v>
+      </c>
+      <c r="K17" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>158.1</v>
+      </c>
+      <c r="M17">
+        <v>46.6</v>
+      </c>
+      <c r="N17">
+        <v>66.3</v>
+      </c>
+      <c r="O17">
+        <v>78.3</v>
+      </c>
+      <c r="P17">
+        <v>53.9</v>
+      </c>
+      <c r="Q17">
+        <v>67.3</v>
+      </c>
+      <c r="R17">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="S17">
+        <v>47.5</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>587.9</v>
+      </c>
+      <c r="W17">
+        <f>SUM(L17:N17,Q17:T17)</f>
+        <v>455.70000000000005</v>
+      </c>
+      <c r="X17">
+        <f>SUM(O17:P17)</f>
+        <v>132.19999999999999</v>
+      </c>
+      <c r="Z17" t="str">
+        <f>G18</f>
+        <v>-</v>
+      </c>
+      <c r="AA17" t="str">
+        <f>H18</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>587.9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="S19" t="s">
+        <v>77</v>
+      </c>
+      <c r="U19" t="s">
+        <v>78</v>
+      </c>
+      <c r="W19">
+        <v>1449.421875</v>
+      </c>
+      <c r="X19">
+        <v>965.8359375</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="S20">
+        <f>U20/12</f>
+        <v>3.0208333333333334E-2</v>
+      </c>
+      <c r="T20">
+        <v>12</v>
+      </c>
+      <c r="U20">
+        <f>O7/$T20/2</f>
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="V20">
+        <f>P7/$T20/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="W20">
+        <f>U20*1000/$W$19*144</f>
+        <v>36.014359173377315</v>
+      </c>
+      <c r="X20">
+        <f>V20*1000/$X$19*144</f>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z20">
+        <f>U20*$T20</f>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AA20">
+        <f>V20*$T20</f>
+        <v>3</v>
+      </c>
+      <c r="AC20">
+        <f>Z20*2</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AD20">
+        <f>AA20*2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T21">
+        <v>11</v>
+      </c>
+      <c r="U21">
+        <f t="shared" ref="U21:V29" si="0">O8/$T21/2</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W21">
+        <f t="shared" ref="W21:W29" si="1">U21*1000/$W$19*144</f>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X21">
+        <f t="shared" ref="X21:X29" si="2">V21*1000/$X$19*144</f>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" ref="Z21:AA29" si="3">U21*$T21</f>
+        <v>4</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC21">
+        <f>Z21*2</f>
+        <v>8</v>
+      </c>
+      <c r="AD21">
+        <f>AA21*2</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <f>11*O16/O15</f>
+        <v>7.9749999999999996</v>
+      </c>
+      <c r="Q22">
+        <f>11*P16/P15</f>
+        <v>8</v>
+      </c>
+      <c r="T22">
+        <v>11</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" ref="AC22:AD29" si="4">Z22*2</f>
+        <v>8</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T23">
+        <v>11</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T24">
+        <v>11</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T25">
+        <v>11</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T26">
+        <v>11</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T27">
+        <v>11</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T28">
+        <v>11</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="1"/>
+        <v>36.127256851036805</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="3"/>
+        <v>2.75</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="T29">
+        <v>8</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="0"/>
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="1"/>
+        <v>36.014359173377315</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="2"/>
+        <v>37.273411148050187</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="3"/>
+        <v>2.9</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="4"/>
+        <v>5.8</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2EE836-5F7D-4255-9C52-1AFACBA37C61}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F1">
         <v>3</v>
       </c>
@@ -2342,45 +4300,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
       </c>
       <c r="G2" s="20"/>
       <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>47</v>
-      </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="10">
         <v>9050</v>
@@ -2432,9 +4390,9 @@
         <v>8.4443519999999967</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10">
         <v>12370</v>
@@ -2486,9 +4444,9 @@
         <v>11.628287999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="10">
         <v>12370</v>
@@ -2540,9 +4498,9 @@
         <v>11.628287999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="10">
         <v>9050</v>
@@ -2594,9 +4552,9 @@
         <v>8.4443519999999967</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="10">
         <v>8560</v>
@@ -2648,9 +4606,9 @@
         <v>1.0690559999999978</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="10">
         <v>13932</v>
@@ -2702,9 +4660,9 @@
         <v>1.7326079999999962</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="10">
         <v>13932</v>
@@ -2756,9 +4714,9 @@
         <v>1.7326079999999962</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10">
         <v>8560</v>
@@ -2810,9 +4768,9 @@
         <v>1.0690559999999978</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="10">
         <v>10442</v>
@@ -2864,9 +4822,9 @@
         <v>-5.507328000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="10">
         <v>10442</v>
@@ -2918,9 +4876,9 @@
         <v>-5.507328000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="10">
         <v>10063</v>
@@ -2972,9 +4930,9 @@
         <v>-8.9466240000000035</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="10">
         <v>9530</v>
@@ -3026,9 +4984,9 @@
         <v>-8.4203520000000029</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="10">
         <v>9530</v>
@@ -3080,9 +5038,9 @@
         <v>-8.4203520000000029</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="10">
         <v>10063</v>
@@ -3134,7 +5092,7 @@
         <v>-8.9466240000000035</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -3159,13 +5117,13 @@
         <v>1.0000000000000002</v>
       </c>
       <c r="K18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="K19">
         <f>SUM(K3:K16)/$G18</f>
         <v>191.99999999999994</v>
@@ -3175,7 +5133,7 @@
         <v>-138.43199999999996</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="M19:P19" si="10">SUM(O3:O16)/$G18</f>
+        <f t="shared" ref="O19:P19" si="10">SUM(O3:O16)/$G18</f>
         <v>5.3290705182007501E-14</v>
       </c>
       <c r="P19">
@@ -3183,9 +5141,9 @@
         <v>-4.0856207306205754E-14</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>